<commit_message>
index for application management page
</commit_message>
<xml_diff>
--- a/public/uploads/excel/student.xlsx
+++ b/public/uploads/excel/student.xlsx
@@ -1,21 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuqin\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50365A8-FC90-4BF7-A0DC-0A608B9D4600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Nama</t>
   </si>
@@ -32,61 +49,98 @@
     <t>No. Tel Bimbit Penjaga</t>
   </si>
   <si>
-    <t>Student 2</t>
+    <t>murid 1</t>
   </si>
   <si>
     <t>L</t>
   </si>
   <si>
-    <t>student2@gmail.com</t>
-  </si>
-  <si>
-    <t>PARENT STUDENT 2</t>
-  </si>
-  <si>
-    <t>0123698654</t>
-  </si>
-  <si>
-    <t>Student 4</t>
-  </si>
-  <si>
-    <t>student4@gmail.com</t>
-  </si>
-  <si>
-    <t>PARENT STUDENT 4</t>
-  </si>
-  <si>
-    <t>0125896647</t>
-  </si>
-  <si>
-    <t>Student 5</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>student5@gmail.com</t>
-  </si>
-  <si>
-    <t>PARENT STUDENT 5</t>
-  </si>
-  <si>
-    <t>0148855796</t>
+    <t>murid1@gmail.com</t>
+  </si>
+  <si>
+    <t>PENJAGA 1</t>
+  </si>
+  <si>
+    <t>murid 2</t>
+  </si>
+  <si>
+    <t>murid 3</t>
+  </si>
+  <si>
+    <t>murid 4</t>
+  </si>
+  <si>
+    <t>murid 5</t>
+  </si>
+  <si>
+    <t>murid 6</t>
+  </si>
+  <si>
+    <t>murid 7</t>
+  </si>
+  <si>
+    <t>murid 8</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>murid2@gmail.com</t>
+  </si>
+  <si>
+    <t>murid3@gmail.com</t>
+  </si>
+  <si>
+    <t>murid4@gmail.com</t>
+  </si>
+  <si>
+    <t>murid5@gmail.com</t>
+  </si>
+  <si>
+    <t>murid6@gmail.com</t>
+  </si>
+  <si>
+    <t>murid7@gmail.com</t>
+  </si>
+  <si>
+    <t>murid8@gmail.com</t>
+  </si>
+  <si>
+    <t>PENJAGA 2</t>
+  </si>
+  <si>
+    <t>PENJAGA 3</t>
+  </si>
+  <si>
+    <t>PENJAGA 4</t>
+  </si>
+  <si>
+    <t>PENJAGA 5</t>
+  </si>
+  <si>
+    <t>PENJAGA 6</t>
+  </si>
+  <si>
+    <t>PENJAGA 7</t>
+  </si>
+  <si>
+    <t>PENJAGA 8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -99,21 +153,36 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -403,26 +472,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="22" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="26" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -452,57 +517,140 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>60989675619</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>60989675610</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>60989675611</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <v>60989675612</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6">
+        <v>60989675613</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7">
+        <v>60989675614</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <v>60989675615</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9">
+        <v>60989675616</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{0E7890CA-D787-49FF-9A77-8FF8204D301D}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{E6A7B4CD-7E34-4DE4-9AB4-7734D415A19C}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{9F7EE840-3472-437A-9DCC-BCE36DCB36EC}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{B436C6AF-7F0E-4EE0-B1A5-DD6C11279C8C}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{6C099507-8616-428D-A502-01E2F4AD6F0D}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{9EC6A637-1B9B-4F63-9A72-DCBB821D7AC4}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{6DE07EF6-D178-437B-BBB9-039F427E1F70}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>